<commit_message>
Pagina das BOOs adicionada ao excel
</commit_message>
<xml_diff>
--- a/Sprint2/USBD11/Dataset normalizado Sem BOO.xlsx
+++ b/Sprint2/USBD11/Dataset normalizado Sem BOO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documentos\bddad2024\Sprint2\USBD11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F89F0AC2-EF03-430B-9C80-A1153042D310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F357275A-0115-46AA-B7E7-0D9F2601CD6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="700" activeTab="7" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="700" firstSheet="2" activeTab="10" xr2:uid="{96054C54-0AC6-4E0E-AB4B-5CA509897BDA}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="228">
   <si>
     <t>Name</t>
   </si>
@@ -468,9 +468,6 @@
     <t>WorkstationTypeId</t>
   </si>
   <si>
-    <t>Operation_SequenceNumber</t>
-  </si>
-  <si>
     <t>PN18324C51</t>
   </si>
   <si>
@@ -724,6 +721,15 @@
   </si>
   <si>
     <t>Handle Gluing</t>
+  </si>
+  <si>
+    <t>OutputId</t>
+  </si>
+  <si>
+    <t>BOOId</t>
+  </si>
+  <si>
+    <t>PartId</t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1152,7 @@
         <v>128</v>
       </c>
       <c r="H1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1163,10 +1169,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1193,10 +1199,10 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1223,10 +1229,10 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -1253,10 +1259,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -1722,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629B436D-7E6F-45CD-A274-6E2AE1A9129E}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1735,270 +1741,89 @@
     <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
         <v>138</v>
       </c>
-      <c r="C1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>125</v>
-      </c>
-      <c r="B2">
-        <v>5647</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="str">
-        <f>"INSERT INTO BOO(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; "," &amp; $C$1 &amp; ") VALUES(" &amp; A2 &amp; ", " &amp; B2 &amp; "," &amp; C2 &amp; ");"</f>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5647,1);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>125</v>
-      </c>
-      <c r="B3">
-        <v>5647</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="str">
-        <f t="shared" ref="E3:E18" si="0">"INSERT INTO BOO(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; "," &amp; $C$1 &amp; ") VALUES(" &amp; A3 &amp; ", " &amp; B3 &amp; "," &amp; C3 &amp; ");"</f>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5647,2);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>125</v>
-      </c>
-      <c r="B4">
-        <v>5649</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5649,3);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>125</v>
-      </c>
-      <c r="B5">
-        <v>5651</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5651,4);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>125</v>
-      </c>
-      <c r="B6">
-        <v>5653</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5653,5);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>125</v>
-      </c>
-      <c r="B7">
-        <v>5659</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5659,6);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>125</v>
-      </c>
-      <c r="B8">
-        <v>5669</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5669,7);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>125</v>
-      </c>
-      <c r="B9">
-        <v>5655</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5655,8);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>125</v>
-      </c>
-      <c r="B10">
-        <v>5657</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5657,9);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>125</v>
-      </c>
-      <c r="B11">
-        <v>5661</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5661,10);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>125</v>
-      </c>
-      <c r="B12">
-        <v>5667</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5667,11);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>125</v>
-      </c>
-      <c r="B13">
-        <v>5663</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="E13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(125, 5663,12);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>132</v>
-      </c>
-      <c r="B14">
-        <v>5681</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="E14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(132, 5681,1);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>132</v>
-      </c>
-      <c r="B15">
-        <v>5682</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="E15" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(132, 5682,2);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>132</v>
-      </c>
-      <c r="B16">
-        <v>5683</v>
-      </c>
-      <c r="C16">
-        <v>3</v>
-      </c>
-      <c r="E16" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(132, 5683,3);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>132</v>
-      </c>
-      <c r="B17">
-        <v>5665</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(132, 5665,4);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>132</v>
-      </c>
-      <c r="B18">
-        <v>5688</v>
-      </c>
-      <c r="C18">
-        <v>5</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO BOO(ProductFamilyId,OperationId,Operation_SequenceNumber) VALUES(132, 5688,5);</v>
+      <c r="D1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" t="str">
+        <f>"INSERT INTO BOO(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; "," &amp; $C$1 &amp; "," &amp; $D$1 &amp; ") VALUES('" &amp; A2 &amp; "', '" &amp; B2 &amp; "', " &amp; C2 &amp; ", '" &amp; D2 &amp; "');"</f>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F10" si="0">"INSERT INTO BOO(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; "," &amp; $C$1 &amp; "," &amp; $D$1 &amp; ") VALUES('" &amp; A3 &amp; "', '" &amp; B3 &amp; "', " &amp; C3 &amp; ", '" &amp; D3 &amp; "');"</f>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO BOO(Id,ProductId,OperationId,OutputId) VALUES('', '', , '');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B19" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="str">
+        <f>"INSERT INTO BOO(" &amp; $A$19 &amp; "," &amp; $B$19 &amp; "," &amp; $C$19 &amp; ") VALUES('" &amp; A20 &amp; "', '" &amp; B20 &amp; "', " &amp; C20 &amp; ");"</f>
+        <v>INSERT INTO BOO(BOOId,PartId,Quantity) VALUES('', '', );</v>
       </c>
     </row>
   </sheetData>
@@ -2032,13 +1857,13 @@
         <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2241,7 +2066,7 @@
         <v>127</v>
       </c>
       <c r="B1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C1" t="s">
         <v>128</v>
@@ -2410,7 +2235,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
         <v>136</v>
@@ -2475,7 +2300,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -2614,7 +2439,7 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23">
         <v>16</v>
@@ -2654,7 +2479,7 @@
         <v>127</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C26" t="s">
         <v>136</v>
@@ -2663,7 +2488,7 @@
         <v>78</v>
       </c>
       <c r="E26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -2738,7 +2563,7 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D30">
         <v>20</v>
@@ -2906,7 +2731,7 @@
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D38">
         <v>16</v>
@@ -2971,7 +2796,7 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" t="str">
         <f>"INSERT INTO ProductFamily(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; ") VALUES(" &amp; A2 &amp; ", '" &amp; B2 &amp; "');"</f>
@@ -2983,7 +2808,7 @@
         <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D7" si="0">"INSERT INTO ProductFamily(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; ") VALUES(" &amp; A3 &amp; ", '" &amp; B3 &amp; "');"</f>
@@ -2995,7 +2820,7 @@
         <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -3007,7 +2832,7 @@
         <v>145</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -3019,7 +2844,7 @@
         <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -3031,7 +2856,7 @@
         <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -3122,7 +2947,7 @@
         <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -3131,7 +2956,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6">
         <v>132</v>
@@ -3176,13 +3001,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9">
         <v>147</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -3191,13 +3016,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10">
         <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -3206,13 +3031,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11">
         <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -3221,13 +3046,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12">
         <v>145</v>
       </c>
       <c r="C12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -3314,7 +3139,7 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -3330,7 +3155,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -3378,7 +3203,7 @@
         <v>INSERT INTO Part(Id,Name) VALUES('AS12945G48','Pro Clear 17 lid');</v>
       </c>
       <c r="O8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q8" t="str">
         <f t="shared" si="1"/>
@@ -3397,7 +3222,7 @@
         <v>INSERT INTO Part(Id,Name) VALUES('PN12344A21','Screw M6 35 mm');</v>
       </c>
       <c r="O9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="Q9" t="str">
         <f t="shared" si="1"/>
@@ -3445,10 +3270,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" t="s">
         <v>141</v>
-      </c>
-      <c r="B13" t="s">
-        <v>142</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -3464,10 +3289,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" t="s">
         <v>177</v>
-      </c>
-      <c r="B14" t="s">
-        <v>178</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -3493,7 +3318,7 @@
         <v>INSERT INTO Part(Id,Name) VALUES('PN52384R50','300x300 mm 5mm stainless steel sheet');</v>
       </c>
       <c r="O15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="2"/>
@@ -3512,7 +3337,7 @@
         <v>INSERT INTO Part(Id,Name) VALUES('PN52384R10','300x300 mm 1mm stainless steel sheet');</v>
       </c>
       <c r="O16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="2"/>
@@ -3521,17 +3346,17 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" t="s">
         <v>167</v>
       </c>
-      <c r="B17" t="s">
-        <v>168</v>
-      </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO Part(Id,Name) VALUES('PN52384R45','250x250 mm 5mm stainless steel sheet');</v>
       </c>
       <c r="O17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="2"/>
@@ -3540,10 +3365,10 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
         <v>169</v>
-      </c>
-      <c r="B18" t="s">
-        <v>170</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -3552,10 +3377,10 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -3564,10 +3389,10 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -3579,17 +3404,17 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO Part(Id,Name) VALUES('AS12946S20','3l 20 cm stainless steel pot bottom');</v>
       </c>
       <c r="O21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q21" t="str">
         <f>"INSERT INTO IntermediateProduct(" &amp; $O$20 &amp; ") VALUES('" &amp; O21 &amp; "');"</f>
@@ -3598,17 +3423,17 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO Part(Id,Name) VALUES('AS12947S20','20 cm stainless steel lid');</v>
       </c>
       <c r="O22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" ref="Q22:Q34" si="3">"INSERT INTO IntermediateProduct(" &amp; $O$20 &amp; ") VALUES('" &amp; O22 &amp; "');"</f>
@@ -3617,17 +3442,17 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12945A01','250 mm 5 mm stailess steel disc');</v>
       </c>
       <c r="O23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="3"/>
@@ -3636,17 +3461,17 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" ref="D24:D37" si="4">"INSERT INTO Part(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; ") VALUES('" &amp; A24 &amp; "','" &amp; B24 &amp; "');"</f>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12945A02','220 mm pot base phase 1');</v>
       </c>
       <c r="O24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="3"/>
@@ -3655,17 +3480,17 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12945A03','220 mm pot base phase 2');</v>
       </c>
       <c r="O25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="3"/>
@@ -3674,17 +3499,17 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12945A04','220 mm pot base final');</v>
       </c>
       <c r="O26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="3"/>
@@ -3693,17 +3518,17 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12947A01','250 mm 1 mm stailess steel disc');</v>
       </c>
       <c r="O27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="3"/>
@@ -3712,17 +3537,17 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12947A02','220 mm lid pressed');</v>
       </c>
       <c r="O28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="3"/>
@@ -3731,17 +3556,17 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12947A03','220 mm lid polished');</v>
       </c>
       <c r="O29" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="3"/>
@@ -3750,17 +3575,17 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12947A04','220 mm lid with handle');</v>
       </c>
       <c r="O30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" si="3"/>
@@ -3769,17 +3594,17 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12945A32','200 mm pot base phase 1');</v>
       </c>
       <c r="O31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="3"/>
@@ -3788,17 +3613,17 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12945A33','200 mm pot base phase 2');</v>
       </c>
       <c r="O32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="3"/>
@@ -3807,17 +3632,17 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12945A34','200 mm pot base final');</v>
       </c>
       <c r="O33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" si="3"/>
@@ -3826,17 +3651,17 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="4"/>
         <v>INSERT INTO Part(Id,Name) VALUES('IP12947A32','200 mm lid pressed');</v>
       </c>
       <c r="O34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" si="3"/>
@@ -3845,10 +3670,10 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="4"/>
@@ -3857,10 +3682,10 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="4"/>
@@ -3869,10 +3694,10 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="4"/>
@@ -3930,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D5" t="str">
         <f>"INSERT INTO Material(" &amp; $A$4 &amp; "," &amp; $B$4 &amp; ") VALUES(" &amp; A5 &amp; ", '" &amp; B5 &amp; "');"</f>
@@ -3942,7 +3767,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ref="D6:D8" si="0">"INSERT INTO Material(" &amp; $A$4 &amp; "," &amp; $B$4 &amp; ") VALUES(" &amp; A6 &amp; ", '" &amp; B6 &amp; "');"</f>
@@ -3954,7 +3779,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -3966,7 +3791,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -3978,7 +3803,7 @@
         <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -3986,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" t="str">
         <f>"INSERT INTO MeasurementUnit(" &amp; $A$10 &amp; "," &amp; $B$10 &amp; ") VALUES(" &amp; A11 &amp; ", '" &amp; B11 &amp; "');"</f>
@@ -3998,7 +3823,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ref="D12:D13" si="1">"INSERT INTO MeasurementUnit(" &amp; $A$10 &amp; "," &amp; $B$10 &amp; ") VALUES(" &amp; A12 &amp; ", '" &amp; B12 &amp; "');"</f>
@@ -4010,7 +3835,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="1"/>
@@ -4022,7 +3847,7 @@
         <v>136</v>
       </c>
       <c r="B16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4036,7 +3861,7 @@
         <v>136</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -4125,7 +3950,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -4137,7 +3962,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B29">
         <v>3</v>
@@ -4149,7 +3974,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B30">
         <v>3</v>
@@ -4161,7 +3986,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -4173,7 +3998,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B32">
         <v>3</v>
@@ -4191,10 +4016,10 @@
         <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E34" t="s">
         <v>14</v>
@@ -4415,7 +4240,7 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -4436,7 +4261,7 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C46">
         <v>17</v>
@@ -4457,7 +4282,7 @@
         <v>13</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C47">
         <v>5</v>
@@ -4478,7 +4303,7 @@
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C48">
         <v>22</v>
@@ -4499,7 +4324,7 @@
         <v>15</v>
       </c>
       <c r="B49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C49">
         <v>22</v>
@@ -4520,7 +4345,7 @@
         <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -4541,7 +4366,7 @@
         <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C51">
         <v>20</v>
@@ -4562,7 +4387,7 @@
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C52">
         <v>20</v>
@@ -4587,7 +4412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8F968F-3FE6-476E-97DD-6EBBFE3BD57E}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D22" sqref="D22:D46"/>
     </sheetView>
   </sheetViews>
@@ -4767,7 +4592,7 @@
         <v>5681</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -4779,7 +4604,7 @@
         <v>5682</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -4791,7 +4616,7 @@
         <v>5683</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -4803,7 +4628,7 @@
         <v>5685</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -4815,7 +4640,7 @@
         <v>5688</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D19" t="str">
         <f>"INSERT INTO Operation(" &amp; $A$1 &amp; "," &amp; $B$1 &amp; ") VALUES(" &amp; A19 &amp; ", '" &amp; B19 &amp; "');"</f>
@@ -5140,7 +4965,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5320,12 +5145,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5562,17 +5386,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C8F835-22B2-4A5C-B33C-2EBD4DAC13D0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7026BE-4F45-4595-B98C-E9D8129D4591}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="c83fef03-7e53-47dc-8a06-28f89aa017e1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5597,18 +5431,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE7026BE-4F45-4595-B98C-E9D8129D4591}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C8F835-22B2-4A5C-B33C-2EBD4DAC13D0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6d3c5dfb-1cc0-4432-86cb-2a9d0e8e17b0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="c83fef03-7e53-47dc-8a06-28f89aa017e1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>